<commit_message>
SVG export for clusters (lists)
</commit_message>
<xml_diff>
--- a/Data/ExploreList2D-SquareSets2to15.xlsx
+++ b/Data/ExploreList2D-SquareSets2to15.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="38115" windowHeight="18210"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="38115" windowHeight="18210" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ExploreList2D-results" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="59">
   <si>
     <t>name</t>
   </si>
@@ -179,6 +180,18 @@
   </si>
   <si>
     <t>/oddErrSum/Pi/2</t>
+  </si>
+  <si>
+    <t>Set</t>
+  </si>
+  <si>
+    <t>Side length</t>
+  </si>
+  <si>
+    <t>N(points)</t>
+  </si>
+  <si>
+    <t>sum of ODD errors</t>
   </si>
 </sst>
 </file>
@@ -1034,11 +1047,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AD19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Z4" sqref="Z4"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2778,4 +2791,232 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>16</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>25</v>
+      </c>
+      <c r="D5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>36</v>
+      </c>
+      <c r="D6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>49</v>
+      </c>
+      <c r="D7">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>64</v>
+      </c>
+      <c r="D8">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>81</v>
+      </c>
+      <c r="D9">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>100</v>
+      </c>
+      <c r="D10">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11">
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <v>121</v>
+      </c>
+      <c r="D11">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>144</v>
+      </c>
+      <c r="D12">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13">
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <v>169</v>
+      </c>
+      <c r="D13">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>196</v>
+      </c>
+      <c r="D14">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15">
+        <v>15</v>
+      </c>
+      <c r="C15">
+        <v>225</v>
+      </c>
+      <c r="D15">
+        <v>1120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>